<commit_message>
WithDraw Deal Testcase Update
</commit_message>
<xml_diff>
--- a/TestData/Deals.xlsx
+++ b/TestData/Deals.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Add Deal" sheetId="1" r:id="rId1"/>
     <sheet name="Deal Widget" sheetId="4" r:id="rId2"/>
+    <sheet name="Duplicate" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="65">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -144,6 +145,72 @@
   </si>
   <si>
     <t>ShareDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>DuplicateDeal_TC001</t>
+  </si>
+  <si>
+    <t>DuplicateDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>DUPLICATE</t>
+  </si>
+  <si>
+    <t>Copies</t>
+  </si>
+  <si>
+    <t>Copies created successfully</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>DuplicateDeal_TC001(3)</t>
+  </si>
+  <si>
+    <t>AutoDeal(1)</t>
+  </si>
+  <si>
+    <t>DuplicateDeal_TC002</t>
+  </si>
+  <si>
+    <t>DuplicateDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>AutoDeal(2)</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC001</t>
+  </si>
+  <si>
+    <t>WITHDRAW</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>WithDraw</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC001(3)</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC002</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC002(3)</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC003</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC003(2)</t>
+  </si>
+  <si>
+    <t>WithDrawDeal_TC003(3)</t>
   </si>
 </sst>
 </file>
@@ -498,15 +565,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -746,6 +813,196 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -754,15 +1011,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
@@ -861,8 +1118,340 @@
         <v>36</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit, ReShare, Discard Deal Testcases
</commit_message>
<xml_diff>
--- a/TestData/Deals.xlsx
+++ b/TestData/Deals.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Add Deal" sheetId="1" r:id="rId1"/>
-    <sheet name="Deal Widget" sheetId="4" r:id="rId2"/>
-    <sheet name="Duplicate" sheetId="5" r:id="rId3"/>
+    <sheet name="Edit Deal" sheetId="6" r:id="rId2"/>
+    <sheet name="Deal Widget" sheetId="4" r:id="rId3"/>
+    <sheet name="Duplicate" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Edit Deal'!$A$1:$N$2</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="93">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -211,6 +215,90 @@
   </si>
   <si>
     <t>WithDrawDeal_TC003(3)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC001</t>
+  </si>
+  <si>
+    <t>EditDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>EDIT</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Edited deal successfully</t>
+  </si>
+  <si>
+    <t>EditDeal_TC001(3)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC002</t>
+  </si>
+  <si>
+    <t>EditDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC002(3)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC003</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>EditDeal_TC003(2)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC003(3)</t>
+  </si>
+  <si>
+    <t>ReShareDeal_TC001</t>
+  </si>
+  <si>
+    <t>ReShareDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>ReShareDeal_TC002</t>
+  </si>
+  <si>
+    <t>ReShareDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>ReShareDeal_TC003</t>
+  </si>
+  <si>
+    <t>ReShareDeal_TC003(2)</t>
+  </si>
+  <si>
+    <t>DiscardDeal_TC001</t>
+  </si>
+  <si>
+    <t>DISCARD</t>
+  </si>
+  <si>
+    <t>DiscardDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>Unable to find Deal</t>
+  </si>
+  <si>
+    <t>DiscardDeal_TC002</t>
+  </si>
+  <si>
+    <t>DiscardDeal_TC003</t>
+  </si>
+  <si>
+    <t>DiscardDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>DiscardDeal_TC003(2)</t>
   </si>
 </sst>
 </file>
@@ -565,10 +653,796 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J4" sqref="J4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,13 +1499,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -639,17 +1513,17 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>10</v>
+      <c r="F2" s="2">
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
@@ -658,18 +1532,18 @@
         <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -677,17 +1551,17 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
-        <v>20</v>
+      <c r="F3" s="2">
+        <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="I3">
-        <v>1</v>
+      <c r="I3" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
@@ -696,18 +1570,18 @@
         <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -715,17 +1589,17 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
-        <v>5</v>
+      <c r="F4" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -734,288 +1608,19 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1390,13 +1995,370 @@
         <v>36</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Edit deal, public share and counter deal Test case update
</commit_message>
<xml_diff>
--- a/TestData/Deals.xlsx
+++ b/TestData/Deals.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Add Deal" sheetId="1" r:id="rId1"/>
     <sheet name="Edit Deal" sheetId="6" r:id="rId2"/>
     <sheet name="Deal Widget" sheetId="4" r:id="rId3"/>
-    <sheet name="Duplicate" sheetId="5" r:id="rId4"/>
+    <sheet name="Counter Deal" sheetId="7" r:id="rId4"/>
+    <sheet name="Duplicate" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Edit Deal'!$A$1:$N$2</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="114">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -79,9 +80,6 @@
     <t>AutoDeal</t>
   </si>
   <si>
-    <t>Ammonia</t>
-  </si>
-  <si>
     <t>Miles (MI)</t>
   </si>
   <si>
@@ -299,13 +297,79 @@
   </si>
   <si>
     <t>DiscardDeal_TC003(2)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC004</t>
+  </si>
+  <si>
+    <t>Cottonseed</t>
+  </si>
+  <si>
+    <t>EditDeal_TC004(2)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC005</t>
+  </si>
+  <si>
+    <t>EditDeal_TC006</t>
+  </si>
+  <si>
+    <t>EditDeal_TC005(2)</t>
+  </si>
+  <si>
+    <t>EditDeal_TC006(2)</t>
+  </si>
+  <si>
+    <t>PublicShareDeal_TC001</t>
+  </si>
+  <si>
+    <t>PublicShareDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>PublicShareDeal_TC002</t>
+  </si>
+  <si>
+    <t>PublicShareDeal_TC003</t>
+  </si>
+  <si>
+    <t>PublicShareDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>PublicShareDeal_TC003(2)</t>
+  </si>
+  <si>
+    <t>CounterDeal_TC001</t>
+  </si>
+  <si>
+    <t>CounterDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Conversation Count</t>
+  </si>
+  <si>
+    <t>San Jose, CA, USA</t>
+  </si>
+  <si>
+    <t>Rate/UOM</t>
+  </si>
+  <si>
+    <t>$ 5.00/ea</t>
+  </si>
+  <si>
+    <t>Countered deal successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +384,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -342,13 +412,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,13 +724,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27:K27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -711,13 +784,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -729,19 +802,19 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
         <v>17</v>
@@ -749,13 +822,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -767,19 +840,19 @@
         <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
         <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s">
         <v>17</v>
@@ -787,13 +860,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -805,19 +878,19 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
         <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
       </c>
       <c r="L4" t="s">
         <v>17</v>
@@ -825,13 +898,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -843,19 +916,19 @@
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
         <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
@@ -863,13 +936,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -881,19 +954,19 @@
         <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
         <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L6" t="s">
         <v>17</v>
@@ -901,13 +974,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -919,19 +992,19 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
         <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" t="s">
         <v>17</v>
@@ -939,13 +1012,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -957,19 +1030,19 @@
         <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
         <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" t="s">
         <v>17</v>
@@ -977,13 +1050,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -995,19 +1068,19 @@
         <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
         <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" t="s">
         <v>17</v>
@@ -1015,13 +1088,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1033,19 +1106,19 @@
         <v>20</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
         <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" t="s">
         <v>17</v>
@@ -1053,13 +1126,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -1071,19 +1144,19 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
         <v>32</v>
-      </c>
-      <c r="K11" t="s">
-        <v>33</v>
       </c>
       <c r="L11" t="s">
         <v>17</v>
@@ -1091,13 +1164,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -1109,19 +1182,19 @@
         <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
         <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L12" t="s">
         <v>17</v>
@@ -1129,13 +1202,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1147,19 +1220,19 @@
         <v>20</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
         <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L13" t="s">
         <v>17</v>
@@ -1167,13 +1240,13 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -1185,19 +1258,19 @@
         <v>5</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" t="s">
         <v>32</v>
-      </c>
-      <c r="K14" t="s">
-        <v>33</v>
       </c>
       <c r="L14" t="s">
         <v>17</v>
@@ -1205,13 +1278,13 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1223,19 +1296,19 @@
         <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
         <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>21</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L15" t="s">
         <v>17</v>
@@ -1243,13 +1316,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1261,19 +1334,19 @@
         <v>5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" t="s">
         <v>32</v>
-      </c>
-      <c r="K16" t="s">
-        <v>33</v>
       </c>
       <c r="L16" t="s">
         <v>17</v>
@@ -1281,13 +1354,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -1299,19 +1372,19 @@
         <v>20</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
         <v>27</v>
-      </c>
-      <c r="H17" t="s">
-        <v>28</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L17" t="s">
         <v>17</v>
@@ -1319,13 +1392,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -1337,19 +1410,19 @@
         <v>10</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" t="s">
         <v>20</v>
-      </c>
-      <c r="H18" t="s">
-        <v>21</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L18" t="s">
         <v>17</v>
@@ -1357,13 +1430,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -1375,19 +1448,19 @@
         <v>20</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
         <v>27</v>
-      </c>
-      <c r="H19" t="s">
-        <v>28</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L19" t="s">
         <v>17</v>
@@ -1395,13 +1468,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -1413,21 +1486,287 @@
         <v>5</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" t="s">
         <v>32</v>
       </c>
-      <c r="K20" t="s">
-        <v>33</v>
-      </c>
       <c r="L20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1439,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:K4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,13 +1838,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1517,33 +1856,33 @@
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
       </c>
       <c r="I2" s="2">
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1555,60 +1894,174 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
         <v>68</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>69</v>
+      <c r="L7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1618,13 +2071,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
@@ -1640,7 +2095,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1657,699 +2112,937 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
-      </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
         <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
         <v>85</v>
       </c>
-      <c r="B37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" t="s">
-        <v>86</v>
-      </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
         <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
         <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2359,6 +3052,122 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2379,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2393,24 +3202,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Counter deal, accept deal and date filter Code updated
</commit_message>
<xml_diff>
--- a/TestData/Deals.xlsx
+++ b/TestData/Deals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Add Deal" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="147">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -372,6 +372,96 @@
   </si>
   <si>
     <t>Deals_Chat_CarrierUser_TC003</t>
+  </si>
+  <si>
+    <t>CounterDeal_TC002</t>
+  </si>
+  <si>
+    <t>CounterDeal_TC003</t>
+  </si>
+  <si>
+    <t>AcceptDeal_TC001</t>
+  </si>
+  <si>
+    <t>AcceptDeal_TC002</t>
+  </si>
+  <si>
+    <t>DateFilter_TC001</t>
+  </si>
+  <si>
+    <t>DateFilter_TC002</t>
+  </si>
+  <si>
+    <t>DateFilter_TC003</t>
+  </si>
+  <si>
+    <t>CounterDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>CounterDeal_TC003(2)</t>
+  </si>
+  <si>
+    <t>AcceptDeal_TC001(2)</t>
+  </si>
+  <si>
+    <t>AcceptDeal_TC001(3)</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>AcceptDeal_TC002(2)</t>
+  </si>
+  <si>
+    <t>AcceptDeal_TC002(3)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC001(2)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC001(3)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC001(4)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC002(2)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC002(3)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC002(4)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC003(2)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC003(3)</t>
+  </si>
+  <si>
+    <t>DateFilter_TC003(4)</t>
+  </si>
+  <si>
+    <t>Texarkana, TX, USA</t>
+  </si>
+  <si>
+    <t>$ 10.00/bu</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>$ 15.00/mi</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>$ 20.00/bu</t>
+  </si>
+  <si>
+    <t>$ 10.00/mi</t>
   </si>
 </sst>
 </file>
@@ -421,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -429,6 +519,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,13 +1834,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1758,13 +1849,13 @@
         <v>7</v>
       </c>
       <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" t="s">
         <v>20</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" t="s">
-        <v>27</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -1781,7 +1872,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -1796,7 +1887,7 @@
         <v>7</v>
       </c>
       <c r="F28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>19</v>
@@ -1805,7 +1896,7 @@
         <v>20</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28" t="s">
         <v>21</v>
@@ -1819,7 +1910,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
@@ -1834,7 +1925,7 @@
         <v>7</v>
       </c>
       <c r="F29">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>19</v>
@@ -1843,7 +1934,7 @@
         <v>20</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" t="s">
         <v>21</v>
@@ -1857,13 +1948,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -1872,16 +1963,16 @@
         <v>7</v>
       </c>
       <c r="F30">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H30" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J30" t="s">
         <v>21</v>
@@ -1890,6 +1981,272 @@
         <v>23</v>
       </c>
       <c r="L30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>20</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K37" t="s">
+        <v>32</v>
+      </c>
+      <c r="L37" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2194,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3493,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
         <v>18</v>
@@ -3153,16 +3510,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
         <v>18</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="E56" t="s">
         <v>35</v>
@@ -3170,7 +3527,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
@@ -3187,7 +3544,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -3204,18 +3561,392 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
       <c r="C59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
         <v>38</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>34</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" t="s">
+        <v>39</v>
+      </c>
+      <c r="D68" t="s">
+        <v>107</v>
+      </c>
+      <c r="E68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72" t="s">
+        <v>107</v>
+      </c>
+      <c r="E72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
+        <v>39</v>
+      </c>
+      <c r="D76" t="s">
+        <v>107</v>
+      </c>
+      <c r="E76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" t="s">
+        <v>39</v>
+      </c>
+      <c r="D77" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" t="s">
+        <v>39</v>
+      </c>
+      <c r="D80" t="s">
+        <v>107</v>
+      </c>
+      <c r="E80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" t="s">
+        <v>39</v>
+      </c>
+      <c r="D81" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3227,10 +3958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3299,7 +4030,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -3316,7 +4047,7 @@
       <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>108</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -3332,6 +4063,182 @@
         <v>112</v>
       </c>
       <c r="N2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="N5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N6" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>